<commit_message>
MLB Final Project w Bugs
</commit_message>
<xml_diff>
--- a/jsd920_class_repo/projects/final_project/MLB Data/mlb_data_2016.xlsx
+++ b/jsd920_class_repo/projects/final_project/MLB Data/mlb_data_2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -526,9 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1438,22 +1436,10 @@
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C32" s="9">
-        <f>AVERAGE(C2:C31)</f>
-        <v>724.8</v>
-      </c>
-      <c r="D32" s="9">
-        <f>AVERAGE(D2:D31)</f>
-        <v>724.8</v>
-      </c>
-      <c r="E32" s="12">
-        <f>AVERAGE(E2:E31)</f>
-        <v>80.900000000000006</v>
-      </c>
-      <c r="F32" s="12">
-        <f>AVERAGE(F2:F31)</f>
-        <v>80.966666666666669</v>
-      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>